<commit_message>
Add Retry Analyzer and Some Extra Fields like name course sem and sgpa
</commit_message>
<xml_diff>
--- a/src/test/resources/rolls.xlsx
+++ b/src/test/resources/rolls.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek\Testing\ResultXtractor\ResultXtractor\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{236DBECB-F9EC-40AC-846F-EAA62355C356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF27C0B-816F-4643-9436-4B8C3E974C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{378487DB-AA21-4191-ACD7-D66AD301E74B}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>RollNumber</t>
   </si>
@@ -45,14 +45,81 @@
     <t>0903CA241009</t>
   </si>
   <si>
-    <t>0903CA2410063</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Course</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>SGPA</t>
+  </si>
+  <si>
+    <t>CGPA</t>
+  </si>
+  <si>
+    <t>0903CA241001</t>
+  </si>
+  <si>
+    <t>0903CA241010</t>
+  </si>
+  <si>
+    <t>0903CA241011</t>
+  </si>
+  <si>
+    <t>0903CA241063</t>
+  </si>
+  <si>
+    <t>ALKA DAS</t>
+  </si>
+  <si>
+    <t>MCA 2 Year</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5.40</t>
+  </si>
+  <si>
+    <t>ATUL TIWARI</t>
+  </si>
+  <si>
+    <t>7.00</t>
+  </si>
+  <si>
+    <t>DEV ARYA</t>
+  </si>
+  <si>
+    <t>6.33</t>
+  </si>
+  <si>
+    <t>DEV LIKHAR</t>
+  </si>
+  <si>
+    <t>6.47</t>
+  </si>
+  <si>
+    <t>DEVESH SINGH SISODIYA</t>
+  </si>
+  <si>
+    <t>6.73</t>
+  </si>
+  <si>
+    <t>SHRUTI GARG</t>
+  </si>
+  <si>
+    <t>6.80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,14 +135,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,20 +142,60 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3B95CD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -105,11 +204,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -118,6 +219,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3B95CD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -426,52 +532,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D47949-9FAD-423C-A4D0-ADBA3BC1B2E8}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.88671875"/>
+    <col min="2" max="2" customWidth="true" width="23.5546875"/>
+    <col min="3" max="3" customWidth="true" width="16.44140625"/>
+    <col min="4" max="4" customWidth="true" width="10.21875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Testing.xml file so that now multiple browser can run in same time
</commit_message>
<xml_diff>
--- a/src/test/resources/rolls.xlsx
+++ b/src/test/resources/rolls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek\Testing\ResultXtractor\ResultXtractor\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF27C0B-816F-4643-9436-4B8C3E974C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C67613-AC94-42DC-8364-046185CB8771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{378487DB-AA21-4191-ACD7-D66AD301E74B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="17">
   <si>
     <t>RollNumber</t>
   </si>
@@ -63,15 +63,6 @@
     <t>0903CA241001</t>
   </si>
   <si>
-    <t>0903CA241010</t>
-  </si>
-  <si>
-    <t>0903CA241011</t>
-  </si>
-  <si>
-    <t>0903CA241063</t>
-  </si>
-  <si>
     <t>ALKA DAS</t>
   </si>
   <si>
@@ -94,24 +85,6 @@
   </si>
   <si>
     <t>6.33</t>
-  </si>
-  <si>
-    <t>DEV LIKHAR</t>
-  </si>
-  <si>
-    <t>6.47</t>
-  </si>
-  <si>
-    <t>DEVESH SINGH SISODIYA</t>
-  </si>
-  <si>
-    <t>6.73</t>
-  </si>
-  <si>
-    <t>SHRUTI GARG</t>
-  </si>
-  <si>
-    <t>6.80</t>
   </si>
 </sst>
 </file>
@@ -119,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +109,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -202,15 +182,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -532,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0D47949-9FAD-423C-A4D0-ADBA3BC1B2E8}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,148 +526,112 @@
     <col min="1" max="1" customWidth="true" width="18.88671875"/>
     <col min="2" max="2" customWidth="true" width="23.5546875"/>
     <col min="3" max="3" customWidth="true" width="16.44140625"/>
-    <col min="4" max="4" customWidth="true" width="10.21875"/>
+    <col min="4" max="4" customWidth="true" width="12.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -790,54 +737,6 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>